<commit_message>
Last Update 26-09-2018 10:55:48.89
</commit_message>
<xml_diff>
--- a/IA-Mark Statements/CS8392-OOPS-IA-2-Marks-Statements.xlsx
+++ b/IA-Mark Statements/CS8392-OOPS-IA-2-Marks-Statements.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="107">
   <si>
     <t xml:space="preserve">KGiSL Institute of Technology </t>
   </si>
@@ -335,16 +335,10 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>ABSENT</t>
-  </si>
-  <si>
     <t>`</t>
   </si>
   <si>
     <t xml:space="preserve"> Statement of Marks - Internal Assesment Exams-II-SEP-2018</t>
-  </si>
-  <si>
-    <t>AB</t>
   </si>
 </sst>
 </file>
@@ -937,6 +931,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1035,21 +1044,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1068,7 +1062,19 @@
     <cellStyle name="Normal 2 6" xfId="11"/>
     <cellStyle name="Normal 2 7" xfId="12"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1373,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D2:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B18" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1388,102 +1394,102 @@
   <sheetData>
     <row r="2" spans="4:8" ht="15.75" thickBot="1"/>
     <row r="3" spans="4:8">
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="4:8">
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="38"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="4:8" ht="15.75" thickBot="1">
-      <c r="D5" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
+      <c r="D5" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="4:8">
       <c r="D6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="61" t="s">
+      <c r="E6" s="29" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="44"/>
+      <c r="H6" s="49"/>
     </row>
     <row r="7" spans="4:8">
       <c r="D7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="30" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="46"/>
+      <c r="H7" s="51"/>
     </row>
     <row r="8" spans="4:8" ht="15.75" thickBot="1">
       <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="63" t="s">
+      <c r="E8" s="31" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="52">
         <v>43361</v>
       </c>
-      <c r="H8" s="48"/>
+      <c r="H8" s="53"/>
     </row>
     <row r="9" spans="4:8">
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="F9" s="58" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="57" t="s">
+      <c r="H9" s="62" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="4:8" ht="15.75" thickBot="1">
-      <c r="D10" s="50"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="54"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="59"/>
       <c r="G10" s="25">
         <v>100</v>
       </c>
-      <c r="H10" s="58"/>
+      <c r="H10" s="63"/>
     </row>
     <row r="11" spans="4:8" ht="20.100000000000001" customHeight="1">
       <c r="D11" s="2">
@@ -1496,7 +1502,7 @@
         <v>26</v>
       </c>
       <c r="G11" s="26">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="H11" s="21" t="s">
         <v>103</v>
@@ -1513,10 +1519,10 @@
         <v>28</v>
       </c>
       <c r="G12" s="26">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -1530,10 +1536,10 @@
         <v>30</v>
       </c>
       <c r="G13" s="26">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -1547,7 +1553,7 @@
         <v>32</v>
       </c>
       <c r="G14" s="26">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="H14" s="21" t="s">
         <v>104</v>
@@ -1564,10 +1570,10 @@
         <v>34</v>
       </c>
       <c r="G15" s="26">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -1581,10 +1587,10 @@
         <v>36</v>
       </c>
       <c r="G16" s="26">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -1615,7 +1621,7 @@
         <v>40</v>
       </c>
       <c r="G18" s="26">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="H18" s="21" t="s">
         <v>103</v>
@@ -1632,7 +1638,7 @@
         <v>42</v>
       </c>
       <c r="G19" s="26">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H19" s="21" t="s">
         <v>104</v>
@@ -1649,7 +1655,7 @@
         <v>44</v>
       </c>
       <c r="G20" s="26">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="H20" s="21" t="s">
         <v>104</v>
@@ -1666,7 +1672,7 @@
         <v>46</v>
       </c>
       <c r="G21" s="26">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="H21" s="21" t="s">
         <v>104</v>
@@ -1683,7 +1689,7 @@
         <v>48</v>
       </c>
       <c r="G22" s="26">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="H22" s="21" t="s">
         <v>104</v>
@@ -1700,7 +1706,7 @@
         <v>50</v>
       </c>
       <c r="G23" s="26">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="H23" s="21" t="s">
         <v>104</v>
@@ -1717,7 +1723,7 @@
         <v>52</v>
       </c>
       <c r="G24" s="26">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H24" s="21" t="s">
         <v>103</v>
@@ -1751,7 +1757,7 @@
         <v>56</v>
       </c>
       <c r="G26" s="26">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="H26" s="21" t="s">
         <v>104</v>
@@ -1768,7 +1774,7 @@
         <v>58</v>
       </c>
       <c r="G27" s="26">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="H27" s="21" t="s">
         <v>103</v>
@@ -1785,7 +1791,7 @@
         <v>60</v>
       </c>
       <c r="G28" s="26">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H28" s="21" t="s">
         <v>103</v>
@@ -1802,7 +1808,7 @@
         <v>62</v>
       </c>
       <c r="G29" s="26">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="H29" s="21" t="s">
         <v>104</v>
@@ -1819,10 +1825,10 @@
         <v>64</v>
       </c>
       <c r="G30" s="26">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -1836,7 +1842,7 @@
         <v>66</v>
       </c>
       <c r="G31" s="26">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="H31" s="21" t="s">
         <v>104</v>
@@ -1853,10 +1859,10 @@
         <v>68</v>
       </c>
       <c r="G32" s="26">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -1870,10 +1876,10 @@
         <v>70</v>
       </c>
       <c r="G33" s="26">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -1887,7 +1893,7 @@
         <v>72</v>
       </c>
       <c r="G34" s="26">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H34" s="21" t="s">
         <v>104</v>
@@ -1904,7 +1910,7 @@
         <v>74</v>
       </c>
       <c r="G35" s="26">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="H35" s="21" t="s">
         <v>103</v>
@@ -1921,10 +1927,10 @@
         <v>76</v>
       </c>
       <c r="G36" s="26">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -1938,7 +1944,7 @@
         <v>78</v>
       </c>
       <c r="G37" s="26">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="H37" s="21" t="s">
         <v>104</v>
@@ -1955,10 +1961,10 @@
         <v>80</v>
       </c>
       <c r="G38" s="26">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -1972,7 +1978,7 @@
         <v>82</v>
       </c>
       <c r="G39" s="26">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="H39" s="21" t="s">
         <v>103</v>
@@ -1989,7 +1995,7 @@
         <v>84</v>
       </c>
       <c r="G40" s="26">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="H40" s="21" t="s">
         <v>104</v>
@@ -2006,7 +2012,7 @@
         <v>86</v>
       </c>
       <c r="G41" s="26">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="H41" s="21" t="s">
         <v>104</v>
@@ -2023,7 +2029,7 @@
         <v>88</v>
       </c>
       <c r="G42" s="26">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H42" s="21" t="s">
         <v>103</v>
@@ -2039,11 +2045,11 @@
       <c r="F43" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G43" s="26" t="s">
-        <v>108</v>
+      <c r="G43" s="26">
+        <v>3</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -2057,10 +2063,10 @@
         <v>92</v>
       </c>
       <c r="G44" s="26">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="4:8" ht="20.100000000000001" customHeight="1">
@@ -2074,7 +2080,7 @@
         <v>94</v>
       </c>
       <c r="G45" s="26">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="H45" s="21" t="s">
         <v>104</v>
@@ -2091,7 +2097,7 @@
         <v>96</v>
       </c>
       <c r="G46" s="26">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="H46" s="21" t="s">
         <v>103</v>
@@ -2108,7 +2114,7 @@
         <v>98</v>
       </c>
       <c r="G47" s="26">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="H47" s="21" t="s">
         <v>103</v>
@@ -2125,10 +2131,10 @@
         <v>100</v>
       </c>
       <c r="G48" s="26">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="H48" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="4:8" ht="20.100000000000001" customHeight="1" thickBot="1">
@@ -2142,55 +2148,55 @@
         <v>102</v>
       </c>
       <c r="G49" s="26">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="H49" s="21" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="50" spans="4:8" ht="15.75">
-      <c r="D50" s="55" t="s">
+      <c r="D50" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="59">
-        <v>15</v>
-      </c>
-      <c r="H50" s="29"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="27">
+        <v>26</v>
+      </c>
+      <c r="H50" s="34"/>
     </row>
     <row r="51" spans="4:8" ht="15.75">
-      <c r="D51" s="27" t="s">
+      <c r="D51" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="60">
-        <v>23</v>
-      </c>
-      <c r="H51" s="30"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="28">
+        <v>13</v>
+      </c>
+      <c r="H51" s="35"/>
     </row>
     <row r="52" spans="4:8" ht="15.75">
-      <c r="D52" s="27" t="s">
+      <c r="D52" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="60">
-        <v>1</v>
-      </c>
-      <c r="H52" s="30"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="28">
+        <v>0</v>
+      </c>
+      <c r="H52" s="35"/>
     </row>
     <row r="53" spans="4:8" ht="15.75">
-      <c r="D53" s="27" t="s">
+      <c r="D53" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="60">
-        <v>40</v>
-      </c>
-      <c r="H53" s="30"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="28">
+        <v>66</v>
+      </c>
+      <c r="H53" s="35"/>
     </row>
     <row r="54" spans="4:8" s="1" customFormat="1">
       <c r="D54" s="17"/>
@@ -2228,7 +2234,7 @@
     </row>
     <row r="62" spans="4:8">
       <c r="D62" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2250,7 +2256,7 @@
     <mergeCell ref="H9:H10"/>
   </mergeCells>
   <conditionalFormatting sqref="G11:G49">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>50</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>